<commit_message>
add processing excel function
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Complex_Translated - empty.xlsx
+++ b/src/main/resources/excel/Complex_Translated - empty.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\repos\Rendr\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38B24E-E668-43DB-8852-0BCBB1916B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF13C140-4B24-4789-B9EF-E88618804C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="19236" windowHeight="8244" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
-    <sheet name="Stock Balance" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
-    <sheet name="Additional Notes (Not Required)" sheetId="5" r:id="rId5"/>
+    <sheet name="Stock Balance" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
+    <sheet name="Additional Notes (Not Required)" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="EQPosnDate">'Stock Balance'!#REF!</definedName>
@@ -1761,6 +1760,81 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1773,9 +1847,6 @@
     <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1788,60 +1859,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="26" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="27" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="41" fillId="38" borderId="28" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="38" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="38" borderId="30" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1859,45 +1897,6 @@
     </xf>
     <xf numFmtId="40" fontId="22" fillId="0" borderId="30" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="26" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="27" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="38" borderId="28" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="38" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="38" borderId="30" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -2479,17 +2478,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2499,10 +2498,10 @@
       <c r="D3" s="3"/>
       <c r="E3" s="6"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="87"/>
+      <c r="H3" s="111"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2512,10 +2511,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="7"/>
       <c r="F4" s="48"/>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="87"/>
+      <c r="H4" s="111"/>
       <c r="I4" s="38"/>
       <c r="J4" s="47"/>
     </row>
@@ -2526,49 +2525,49 @@
       <c r="D5" s="49"/>
       <c r="E5" s="50"/>
       <c r="F5" s="72"/>
-      <c r="G5" s="87" t="s">
+      <c r="G5" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="87"/>
+      <c r="H5" s="111"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:15" ht="14.4" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="120" t="s">
+      <c r="B7" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80" t="s">
+      <c r="F7" s="105"/>
+      <c r="G7" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="83" t="s">
+      <c r="H7" s="105"/>
+      <c r="I7" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="85" t="s">
+      <c r="J7" s="109" t="s">
         <v>54</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="88" t="s">
+      <c r="L7" s="98" t="s">
         <v>45</v>
       </c>
       <c r="N7" s="67"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="121"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="107"/>
       <c r="E8" s="13" t="s">
         <v>51</v>
       </c>
@@ -2581,10 +2580,10 @@
       <c r="H8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="86"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="110"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="89"/>
+      <c r="L8" s="99"/>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" s="51">
@@ -2717,20 +2716,20 @@
       <c r="I18" s="37"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="90"/>
+      <c r="C20" s="97"/>
       <c r="I20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J20" s="70"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="92"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="59"/>
       <c r="E21" s="8"/>
       <c r="I21" s="21" t="s">
@@ -2739,10 +2738,10 @@
       <c r="J21" s="60"/>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="94"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="55"/>
       <c r="E22" s="8"/>
       <c r="I22" s="10" t="s">
@@ -2751,10 +2750,10 @@
       <c r="J22" s="61"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="94"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="55"/>
       <c r="I23" s="10" t="s">
         <v>40</v>
@@ -2762,10 +2761,10 @@
       <c r="J23" s="61"/>
     </row>
     <row r="24" spans="2:11" ht="14.4" thickBot="1">
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="100"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="62"/>
       <c r="I24" s="11" t="s">
         <v>31</v>
@@ -2774,28 +2773,28 @@
       <c r="K24" s="69"/>
     </row>
     <row r="27" spans="2:11" ht="14.4" thickBot="1">
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
     </row>
     <row r="28" spans="2:11" ht="41.4">
-      <c r="B28" s="101"/>
-      <c r="C28" s="102"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83" t="s">
+      <c r="F28" s="86"/>
+      <c r="G28" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="95"/>
+      <c r="H28" s="87"/>
       <c r="I28" s="73" t="s">
         <v>43</v>
       </c>
@@ -2804,15 +2803,15 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="14.4" thickBot="1">
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="104"/>
+      <c r="C29" s="96"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="96"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="88"/>
       <c r="I29" s="18">
         <f>E29 - D29</f>
         <v>0</v>
@@ -2828,10 +2827,10 @@
       <c r="J30" s="69"/>
     </row>
     <row r="31" spans="2:11" ht="14.4" thickBot="1">
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="98"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="22"/>
       <c r="G31" s="32"/>
     </row>
@@ -2861,6 +2860,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="B31:C31"/>
@@ -2870,20 +2883,6 @@
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -2895,18 +2894,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AEF94D-985A-4661-914F-4490C662E304}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
@@ -2914,7 +2901,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3097,31 +3084,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449881BD-6A68-49C0-AA20-83DAB95B90EE}">
   <dimension ref="D7:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData>
     <row r="7" spans="4:12" ht="13.8" thickBot="1"/>
     <row r="8" spans="4:12" ht="14.4" customHeight="1" thickBot="1">
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
     </row>
     <row r="9" spans="4:12" ht="96.6">
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="118" t="s">
+      <c r="E9" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="122" t="s">
+      <c r="F9" s="83" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -3136,10 +3123,10 @@
       <c r="J9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="123" t="s">
+      <c r="K9" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="124" t="s">
+      <c r="L9" s="85" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3152,7 +3139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -3167,13 +3154,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="112" t="s">
@@ -3230,190 +3217,200 @@
       <c r="E7" s="114"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="108"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="121"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="115" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="107"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="108"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="121"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="105" t="s">
+      <c r="B18" s="115" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="111"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="124"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="105" t="s">
+      <c r="B24" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B18:E18"/>
@@ -3428,37 +3425,12 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3572,17 +3544,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3596,17 +3584,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>